<commit_message>
lettre de motivation + CV
</commit_message>
<xml_diff>
--- a/Recherche_stage_briantoAlexandre.xlsx
+++ b/Recherche_stage_briantoAlexandre.xlsx
@@ -8,8 +8,8 @@
     <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="STAGE-RECHERCHE-SUIVI" sheetId="1" state="visible" r:id="rId3"/>
-    <sheet name="Listes-menu" sheetId="2" state="visible" r:id="rId4"/>
+    <sheet name="STAGE-RECHERCHE-SUIVI" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="Listes-menu" sheetId="2" state="visible" r:id="rId3"/>
   </sheets>
   <definedNames>
     <definedName function="false" hidden="false" name="reponse" vbProcedure="false">'Listes-menu'!$A$4:$A$6</definedName>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="37">
   <si>
     <t xml:space="preserve">NOM :</t>
   </si>
@@ -120,6 +120,18 @@
     <t xml:space="preserve">oui</t>
   </si>
   <si>
+    <t xml:space="preserve">Enedis</t>
+  </si>
+  <si>
+    <t xml:space="preserve">??</t>
+  </si>
+  <si>
+    <t xml:space="preserve">e.bregnard@courtepaille.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">??/02/2026</t>
+  </si>
+  <si>
     <t xml:space="preserve">positive</t>
   </si>
   <si>
@@ -137,7 +149,7 @@
   <fonts count="9">
     <font>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
@@ -160,28 +172,28 @@
     <font>
       <u val="single"/>
       <sz val="11"/>
-      <color theme="10"/>
+      <color rgb="FF0563C1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF000000"/>
       <name val="Times New Roman"/>
       <family val="1"/>
       <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
-      <color theme="10"/>
+      <color rgb="FF0563C1"/>
       <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="0"/>
     </font>
@@ -201,7 +213,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.7999"/>
+        <fgColor rgb="FFDEEBF7"/>
         <bgColor rgb="FFCCFFFF"/>
       </patternFill>
     </fill>
@@ -331,7 +343,7 @@
     <dxf>
       <fill>
         <patternFill patternType="solid">
-          <bgColor rgb="FF000000"/>
+          <fgColor rgb="00FFFFFF"/>
         </patternFill>
       </fill>
     </dxf>
@@ -339,7 +351,7 @@
       <fill>
         <patternFill patternType="solid">
           <fgColor rgb="FF000000"/>
-          <bgColor rgb="FF000000"/>
+          <bgColor rgb="FFFFFFFF"/>
         </patternFill>
       </fill>
     </dxf>
@@ -347,7 +359,6 @@
       <fill>
         <patternFill patternType="solid">
           <fgColor rgb="FF0563C1"/>
-          <bgColor rgb="FF000000"/>
         </patternFill>
       </fill>
     </dxf>
@@ -426,9 +437,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>16920</xdr:colOff>
+      <xdr:colOff>16560</xdr:colOff>
       <xdr:row>7</xdr:row>
-      <xdr:rowOff>180000</xdr:rowOff>
+      <xdr:rowOff>179640</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -438,7 +449,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="7990200" y="0"/>
-          <a:ext cx="7824240" cy="1513440"/>
+          <a:ext cx="7823880" cy="1513080"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -602,187 +613,15 @@
 </table>
 </file>
 
-<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Office Theme">
-  <a:themeElements>
-    <a:clrScheme name="Office">
-      <a:dk1>
-        <a:srgbClr val="000000"/>
-      </a:dk1>
-      <a:lt1>
-        <a:srgbClr val="ffffff"/>
-      </a:lt1>
-      <a:dk2>
-        <a:srgbClr val="44546a"/>
-      </a:dk2>
-      <a:lt2>
-        <a:srgbClr val="e7e6e6"/>
-      </a:lt2>
-      <a:accent1>
-        <a:srgbClr val="5b9bd5"/>
-      </a:accent1>
-      <a:accent2>
-        <a:srgbClr val="ed7d31"/>
-      </a:accent2>
-      <a:accent3>
-        <a:srgbClr val="a5a5a5"/>
-      </a:accent3>
-      <a:accent4>
-        <a:srgbClr val="ffc000"/>
-      </a:accent4>
-      <a:accent5>
-        <a:srgbClr val="4472c4"/>
-      </a:accent5>
-      <a:accent6>
-        <a:srgbClr val="70ad47"/>
-      </a:accent6>
-      <a:hlink>
-        <a:srgbClr val="0563c1"/>
-      </a:hlink>
-      <a:folHlink>
-        <a:srgbClr val="954f72"/>
-      </a:folHlink>
-    </a:clrScheme>
-    <a:fontScheme name="Office">
-      <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204" pitchFamily="0" charset="1"/>
-        <a:ea typeface=""/>
-        <a:cs typeface=""/>
-      </a:majorFont>
-      <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204" pitchFamily="0" charset="1"/>
-        <a:ea typeface=""/>
-        <a:cs typeface=""/>
-      </a:minorFont>
-    </a:fontScheme>
-    <a:fmtScheme>
-      <a:fillStyleLst>
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:gradFill>
-          <a:gsLst>
-            <a:gs pos="0">
-              <a:schemeClr val="phClr">
-                <a:lumMod val="110000"/>
-                <a:tint val="67000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="50000">
-              <a:schemeClr val="phClr">
-                <a:lumMod val="105000"/>
-                <a:tint val="73000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="100000">
-              <a:schemeClr val="phClr">
-                <a:lumMod val="105000"/>
-                <a:tint val="81000"/>
-              </a:schemeClr>
-            </a:gs>
-          </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
-          <a:tileRect l="0" t="0" r="0" b="0"/>
-        </a:gradFill>
-        <a:gradFill>
-          <a:gsLst>
-            <a:gs pos="0">
-              <a:schemeClr val="phClr">
-                <a:lumMod val="102000"/>
-                <a:tint val="94000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="50000">
-              <a:schemeClr val="phClr">
-                <a:lumMod val="100000"/>
-                <a:shade val="100000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="100000">
-              <a:schemeClr val="phClr">
-                <a:lumMod val="99000"/>
-                <a:shade val="78000"/>
-              </a:schemeClr>
-            </a:gs>
-          </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
-          <a:tileRect l="0" t="0" r="0" b="0"/>
-        </a:gradFill>
-      </a:fillStyleLst>
-      <a:lnStyleLst>
-        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
-          <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
-        </a:ln>
-        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
-          <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
-        </a:ln>
-        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
-          <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
-        </a:ln>
-      </a:lnStyleLst>
-      <a:effectStyleLst>
-        <a:effectStyle>
-          <a:effectLst/>
-        </a:effectStyle>
-        <a:effectStyle>
-          <a:effectLst/>
-        </a:effectStyle>
-        <a:effectStyle>
-          <a:effectLst/>
-        </a:effectStyle>
-      </a:effectStyleLst>
-      <a:bgFillStyleLst>
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:solidFill>
-          <a:schemeClr val="phClr">
-            <a:tint val="95000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:gradFill>
-          <a:gsLst>
-            <a:gs pos="0">
-              <a:schemeClr val="phClr">
-                <a:tint val="93000"/>
-                <a:shade val="98000"/>
-                <a:lumMod val="102000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="50000">
-              <a:schemeClr val="phClr">
-                <a:tint val="98000"/>
-                <a:shade val="90000"/>
-                <a:lumMod val="103000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="100000">
-              <a:schemeClr val="phClr">
-                <a:shade val="63000"/>
-              </a:schemeClr>
-            </a:gs>
-          </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
-          <a:tileRect l="0" t="0" r="0" b="0"/>
-        </a:gradFill>
-      </a:bgFillStyleLst>
-    </a:fmtScheme>
-  </a:themeElements>
-</a:theme>
-</file>
-
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A2:Q256"/>
+  <dimension ref="A2:P256"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B12" activeCellId="0" sqref="B12"/>
+      <selection pane="topLeft" activeCell="C13" activeCellId="0" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.6796875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -938,11 +777,25 @@
         <v>30</v>
       </c>
     </row>
-    <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C13" s="6"/>
-      <c r="D13" s="8"/>
-      <c r="E13" s="6"/>
-      <c r="F13" s="9"/>
+    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C13" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="D13" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="E13" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="F13" s="9" t="s">
+        <v>34</v>
+      </c>
       <c r="G13" s="9"/>
       <c r="H13" s="9"/>
       <c r="I13" s="9"/>
@@ -1351,7 +1204,6 @@
       <c r="N53" s="9"/>
       <c r="O53" s="9"/>
       <c r="P53" s="9"/>
-      <c r="Q53" s="9"/>
     </row>
     <row r="54" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C54" s="6"/>
@@ -1366,7 +1218,6 @@
       <c r="N54" s="9"/>
       <c r="O54" s="9"/>
       <c r="P54" s="9"/>
-      <c r="Q54" s="9"/>
     </row>
     <row r="55" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C55" s="6"/>
@@ -1381,7 +1232,6 @@
       <c r="N55" s="9"/>
       <c r="O55" s="9"/>
       <c r="P55" s="9"/>
-      <c r="Q55" s="9"/>
     </row>
     <row r="56" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C56" s="6"/>
@@ -1396,7 +1246,6 @@
       <c r="N56" s="9"/>
       <c r="O56" s="9"/>
       <c r="P56" s="9"/>
-      <c r="Q56" s="9"/>
     </row>
     <row r="57" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C57" s="6"/>
@@ -1411,7 +1260,6 @@
       <c r="N57" s="9"/>
       <c r="O57" s="9"/>
       <c r="P57" s="9"/>
-      <c r="Q57" s="9"/>
     </row>
     <row r="58" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C58" s="6"/>
@@ -1426,7 +1274,6 @@
       <c r="N58" s="9"/>
       <c r="O58" s="9"/>
       <c r="P58" s="9"/>
-      <c r="Q58" s="9"/>
     </row>
     <row r="59" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C59" s="6"/>
@@ -1441,7 +1288,6 @@
       <c r="N59" s="9"/>
       <c r="O59" s="9"/>
       <c r="P59" s="9"/>
-      <c r="Q59" s="9"/>
     </row>
     <row r="60" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C60" s="6"/>
@@ -1456,7 +1302,6 @@
       <c r="N60" s="9"/>
       <c r="O60" s="9"/>
       <c r="P60" s="9"/>
-      <c r="Q60" s="9"/>
     </row>
     <row r="61" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C61" s="6"/>
@@ -1471,7 +1316,6 @@
       <c r="N61" s="9"/>
       <c r="O61" s="9"/>
       <c r="P61" s="9"/>
-      <c r="Q61" s="9"/>
     </row>
     <row r="62" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C62" s="6"/>
@@ -1486,7 +1330,6 @@
       <c r="N62" s="9"/>
       <c r="O62" s="9"/>
       <c r="P62" s="9"/>
-      <c r="Q62" s="9"/>
     </row>
     <row r="63" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C63" s="6"/>
@@ -1501,7 +1344,6 @@
       <c r="N63" s="9"/>
       <c r="O63" s="9"/>
       <c r="P63" s="9"/>
-      <c r="Q63" s="9"/>
     </row>
     <row r="64" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C64" s="6"/>
@@ -1516,7 +1358,6 @@
       <c r="N64" s="9"/>
       <c r="O64" s="9"/>
       <c r="P64" s="9"/>
-      <c r="Q64" s="9"/>
     </row>
     <row r="65" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C65" s="6"/>
@@ -1531,7 +1372,6 @@
       <c r="N65" s="9"/>
       <c r="O65" s="9"/>
       <c r="P65" s="9"/>
-      <c r="Q65" s="9"/>
     </row>
     <row r="66" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C66" s="6"/>
@@ -1546,7 +1386,6 @@
       <c r="N66" s="9"/>
       <c r="O66" s="9"/>
       <c r="P66" s="9"/>
-      <c r="Q66" s="9"/>
     </row>
     <row r="67" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C67" s="6"/>
@@ -1561,7 +1400,6 @@
       <c r="N67" s="9"/>
       <c r="O67" s="9"/>
       <c r="P67" s="9"/>
-      <c r="Q67" s="9"/>
     </row>
     <row r="68" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C68" s="6"/>
@@ -1576,7 +1414,6 @@
       <c r="N68" s="9"/>
       <c r="O68" s="9"/>
       <c r="P68" s="9"/>
-      <c r="Q68" s="9"/>
     </row>
     <row r="69" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C69" s="6"/>
@@ -1591,7 +1428,6 @@
       <c r="N69" s="9"/>
       <c r="O69" s="9"/>
       <c r="P69" s="9"/>
-      <c r="Q69" s="9"/>
     </row>
     <row r="70" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C70" s="6"/>
@@ -1606,7 +1442,6 @@
       <c r="N70" s="9"/>
       <c r="O70" s="9"/>
       <c r="P70" s="9"/>
-      <c r="Q70" s="9"/>
     </row>
     <row r="71" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C71" s="6"/>
@@ -1621,7 +1456,6 @@
       <c r="N71" s="9"/>
       <c r="O71" s="9"/>
       <c r="P71" s="9"/>
-      <c r="Q71" s="9"/>
     </row>
     <row r="72" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C72" s="6"/>
@@ -1636,7 +1470,6 @@
       <c r="N72" s="9"/>
       <c r="O72" s="9"/>
       <c r="P72" s="9"/>
-      <c r="Q72" s="9"/>
     </row>
     <row r="73" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C73" s="6"/>
@@ -1651,7 +1484,6 @@
       <c r="N73" s="9"/>
       <c r="O73" s="9"/>
       <c r="P73" s="9"/>
-      <c r="Q73" s="9"/>
     </row>
     <row r="74" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C74" s="6"/>
@@ -1666,7 +1498,6 @@
       <c r="N74" s="9"/>
       <c r="O74" s="9"/>
       <c r="P74" s="9"/>
-      <c r="Q74" s="9"/>
     </row>
     <row r="75" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C75" s="6"/>
@@ -1681,7 +1512,6 @@
       <c r="N75" s="9"/>
       <c r="O75" s="9"/>
       <c r="P75" s="9"/>
-      <c r="Q75" s="9"/>
     </row>
     <row r="76" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C76" s="6"/>
@@ -1696,7 +1526,6 @@
       <c r="N76" s="9"/>
       <c r="O76" s="9"/>
       <c r="P76" s="9"/>
-      <c r="Q76" s="9"/>
     </row>
     <row r="77" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C77" s="6"/>
@@ -1711,7 +1540,6 @@
       <c r="N77" s="9"/>
       <c r="O77" s="9"/>
       <c r="P77" s="9"/>
-      <c r="Q77" s="9"/>
     </row>
     <row r="78" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C78" s="6"/>
@@ -1726,7 +1554,6 @@
       <c r="N78" s="9"/>
       <c r="O78" s="9"/>
       <c r="P78" s="9"/>
-      <c r="Q78" s="9"/>
     </row>
     <row r="79" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C79" s="6"/>
@@ -1741,7 +1568,6 @@
       <c r="N79" s="9"/>
       <c r="O79" s="9"/>
       <c r="P79" s="9"/>
-      <c r="Q79" s="9"/>
     </row>
     <row r="80" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C80" s="6"/>
@@ -1756,7 +1582,6 @@
       <c r="N80" s="9"/>
       <c r="O80" s="9"/>
       <c r="P80" s="9"/>
-      <c r="Q80" s="9"/>
     </row>
     <row r="81" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C81" s="6"/>
@@ -1771,7 +1596,6 @@
       <c r="N81" s="9"/>
       <c r="O81" s="9"/>
       <c r="P81" s="9"/>
-      <c r="Q81" s="9"/>
     </row>
     <row r="82" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C82" s="6"/>
@@ -1786,7 +1610,6 @@
       <c r="N82" s="9"/>
       <c r="O82" s="9"/>
       <c r="P82" s="9"/>
-      <c r="Q82" s="9"/>
     </row>
     <row r="83" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C83" s="6"/>
@@ -1801,7 +1624,6 @@
       <c r="N83" s="9"/>
       <c r="O83" s="9"/>
       <c r="P83" s="9"/>
-      <c r="Q83" s="9"/>
     </row>
     <row r="84" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C84" s="6"/>
@@ -1816,7 +1638,6 @@
       <c r="N84" s="9"/>
       <c r="O84" s="9"/>
       <c r="P84" s="9"/>
-      <c r="Q84" s="9"/>
     </row>
     <row r="85" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C85" s="6"/>
@@ -1831,7 +1652,6 @@
       <c r="N85" s="9"/>
       <c r="O85" s="9"/>
       <c r="P85" s="9"/>
-      <c r="Q85" s="9"/>
     </row>
     <row r="86" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C86" s="6"/>
@@ -1846,7 +1666,6 @@
       <c r="N86" s="9"/>
       <c r="O86" s="9"/>
       <c r="P86" s="9"/>
-      <c r="Q86" s="9"/>
     </row>
     <row r="87" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C87" s="6"/>
@@ -1861,7 +1680,6 @@
       <c r="N87" s="9"/>
       <c r="O87" s="9"/>
       <c r="P87" s="9"/>
-      <c r="Q87" s="9"/>
     </row>
     <row r="88" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C88" s="6"/>
@@ -1876,7 +1694,6 @@
       <c r="N88" s="9"/>
       <c r="O88" s="9"/>
       <c r="P88" s="9"/>
-      <c r="Q88" s="9"/>
     </row>
     <row r="89" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C89" s="6"/>
@@ -1891,7 +1708,6 @@
       <c r="N89" s="9"/>
       <c r="O89" s="9"/>
       <c r="P89" s="9"/>
-      <c r="Q89" s="9"/>
     </row>
     <row r="90" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C90" s="6"/>
@@ -1906,7 +1722,6 @@
       <c r="N90" s="9"/>
       <c r="O90" s="9"/>
       <c r="P90" s="9"/>
-      <c r="Q90" s="9"/>
     </row>
     <row r="91" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C91" s="6"/>
@@ -1921,7 +1736,6 @@
       <c r="N91" s="9"/>
       <c r="O91" s="9"/>
       <c r="P91" s="9"/>
-      <c r="Q91" s="9"/>
     </row>
     <row r="92" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C92" s="6"/>
@@ -1936,7 +1750,6 @@
       <c r="N92" s="9"/>
       <c r="O92" s="9"/>
       <c r="P92" s="9"/>
-      <c r="Q92" s="9"/>
     </row>
     <row r="93" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C93" s="6"/>
@@ -1951,7 +1764,6 @@
       <c r="N93" s="9"/>
       <c r="O93" s="9"/>
       <c r="P93" s="9"/>
-      <c r="Q93" s="9"/>
     </row>
     <row r="94" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C94" s="6"/>
@@ -1966,7 +1778,6 @@
       <c r="N94" s="9"/>
       <c r="O94" s="9"/>
       <c r="P94" s="9"/>
-      <c r="Q94" s="9"/>
     </row>
     <row r="95" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C95" s="6"/>
@@ -1981,7 +1792,6 @@
       <c r="N95" s="9"/>
       <c r="O95" s="9"/>
       <c r="P95" s="9"/>
-      <c r="Q95" s="9"/>
     </row>
     <row r="96" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C96" s="6"/>
@@ -1996,7 +1806,6 @@
       <c r="N96" s="9"/>
       <c r="O96" s="9"/>
       <c r="P96" s="9"/>
-      <c r="Q96" s="9"/>
     </row>
     <row r="97" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C97" s="6"/>
@@ -2011,7 +1820,6 @@
       <c r="N97" s="9"/>
       <c r="O97" s="9"/>
       <c r="P97" s="9"/>
-      <c r="Q97" s="9"/>
     </row>
     <row r="98" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C98" s="6"/>
@@ -2026,7 +1834,6 @@
       <c r="N98" s="9"/>
       <c r="O98" s="9"/>
       <c r="P98" s="9"/>
-      <c r="Q98" s="9"/>
     </row>
     <row r="99" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C99" s="6"/>
@@ -2041,7 +1848,6 @@
       <c r="N99" s="9"/>
       <c r="O99" s="9"/>
       <c r="P99" s="9"/>
-      <c r="Q99" s="9"/>
     </row>
     <row r="100" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C100" s="6"/>
@@ -2056,7 +1862,6 @@
       <c r="N100" s="9"/>
       <c r="O100" s="9"/>
       <c r="P100" s="9"/>
-      <c r="Q100" s="9"/>
     </row>
     <row r="101" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C101" s="6"/>
@@ -2071,7 +1876,6 @@
       <c r="N101" s="9"/>
       <c r="O101" s="9"/>
       <c r="P101" s="9"/>
-      <c r="Q101" s="9"/>
     </row>
     <row r="102" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C102" s="6"/>
@@ -2086,7 +1890,6 @@
       <c r="N102" s="9"/>
       <c r="O102" s="9"/>
       <c r="P102" s="9"/>
-      <c r="Q102" s="9"/>
     </row>
     <row r="103" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C103" s="6"/>
@@ -2101,7 +1904,6 @@
       <c r="N103" s="9"/>
       <c r="O103" s="9"/>
       <c r="P103" s="9"/>
-      <c r="Q103" s="9"/>
     </row>
     <row r="104" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C104" s="6"/>
@@ -2116,7 +1918,6 @@
       <c r="N104" s="9"/>
       <c r="O104" s="9"/>
       <c r="P104" s="9"/>
-      <c r="Q104" s="9"/>
     </row>
     <row r="105" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C105" s="6"/>
@@ -2131,7 +1932,6 @@
       <c r="N105" s="9"/>
       <c r="O105" s="9"/>
       <c r="P105" s="9"/>
-      <c r="Q105" s="9"/>
     </row>
     <row r="106" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C106" s="6"/>
@@ -2146,7 +1946,6 @@
       <c r="N106" s="9"/>
       <c r="O106" s="9"/>
       <c r="P106" s="9"/>
-      <c r="Q106" s="9"/>
     </row>
     <row r="107" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C107" s="6"/>
@@ -2161,7 +1960,6 @@
       <c r="N107" s="9"/>
       <c r="O107" s="9"/>
       <c r="P107" s="9"/>
-      <c r="Q107" s="9"/>
     </row>
     <row r="108" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C108" s="6"/>
@@ -2176,7 +1974,6 @@
       <c r="N108" s="9"/>
       <c r="O108" s="9"/>
       <c r="P108" s="9"/>
-      <c r="Q108" s="9"/>
     </row>
     <row r="109" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C109" s="6"/>
@@ -2191,7 +1988,6 @@
       <c r="N109" s="9"/>
       <c r="O109" s="9"/>
       <c r="P109" s="9"/>
-      <c r="Q109" s="9"/>
     </row>
     <row r="110" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C110" s="6"/>
@@ -2206,7 +2002,6 @@
       <c r="N110" s="9"/>
       <c r="O110" s="9"/>
       <c r="P110" s="9"/>
-      <c r="Q110" s="9"/>
     </row>
     <row r="111" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C111" s="6"/>
@@ -2221,7 +2016,6 @@
       <c r="N111" s="9"/>
       <c r="O111" s="9"/>
       <c r="P111" s="9"/>
-      <c r="Q111" s="9"/>
     </row>
     <row r="112" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C112" s="6"/>
@@ -2236,7 +2030,6 @@
       <c r="N112" s="9"/>
       <c r="O112" s="9"/>
       <c r="P112" s="9"/>
-      <c r="Q112" s="9"/>
     </row>
     <row r="113" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C113" s="6"/>
@@ -2251,7 +2044,6 @@
       <c r="N113" s="9"/>
       <c r="O113" s="9"/>
       <c r="P113" s="9"/>
-      <c r="Q113" s="9"/>
     </row>
     <row r="114" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C114" s="6"/>
@@ -2266,7 +2058,6 @@
       <c r="N114" s="9"/>
       <c r="O114" s="9"/>
       <c r="P114" s="9"/>
-      <c r="Q114" s="9"/>
     </row>
     <row r="115" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C115" s="6"/>
@@ -2281,7 +2072,6 @@
       <c r="N115" s="9"/>
       <c r="O115" s="9"/>
       <c r="P115" s="9"/>
-      <c r="Q115" s="9"/>
     </row>
     <row r="116" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C116" s="6"/>
@@ -2296,7 +2086,6 @@
       <c r="N116" s="9"/>
       <c r="O116" s="9"/>
       <c r="P116" s="9"/>
-      <c r="Q116" s="9"/>
     </row>
     <row r="117" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C117" s="6"/>
@@ -2311,7 +2100,6 @@
       <c r="N117" s="9"/>
       <c r="O117" s="9"/>
       <c r="P117" s="9"/>
-      <c r="Q117" s="9"/>
     </row>
     <row r="118" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C118" s="6"/>
@@ -2326,7 +2114,6 @@
       <c r="N118" s="9"/>
       <c r="O118" s="9"/>
       <c r="P118" s="9"/>
-      <c r="Q118" s="9"/>
     </row>
     <row r="119" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C119" s="6"/>
@@ -2341,7 +2128,6 @@
       <c r="N119" s="9"/>
       <c r="O119" s="9"/>
       <c r="P119" s="9"/>
-      <c r="Q119" s="9"/>
     </row>
     <row r="120" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C120" s="6"/>
@@ -2356,7 +2142,6 @@
       <c r="N120" s="9"/>
       <c r="O120" s="9"/>
       <c r="P120" s="9"/>
-      <c r="Q120" s="9"/>
     </row>
     <row r="121" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C121" s="6"/>
@@ -2371,7 +2156,6 @@
       <c r="N121" s="9"/>
       <c r="O121" s="9"/>
       <c r="P121" s="9"/>
-      <c r="Q121" s="9"/>
     </row>
     <row r="122" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C122" s="6"/>
@@ -2386,7 +2170,6 @@
       <c r="N122" s="9"/>
       <c r="O122" s="9"/>
       <c r="P122" s="9"/>
-      <c r="Q122" s="9"/>
     </row>
     <row r="123" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C123" s="6"/>
@@ -2401,7 +2184,6 @@
       <c r="N123" s="9"/>
       <c r="O123" s="9"/>
       <c r="P123" s="9"/>
-      <c r="Q123" s="9"/>
     </row>
     <row r="124" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C124" s="6"/>
@@ -2416,7 +2198,6 @@
       <c r="N124" s="9"/>
       <c r="O124" s="9"/>
       <c r="P124" s="9"/>
-      <c r="Q124" s="9"/>
     </row>
     <row r="125" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C125" s="6"/>
@@ -2431,7 +2212,6 @@
       <c r="N125" s="9"/>
       <c r="O125" s="9"/>
       <c r="P125" s="9"/>
-      <c r="Q125" s="9"/>
     </row>
     <row r="126" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C126" s="6"/>
@@ -2446,7 +2226,6 @@
       <c r="N126" s="9"/>
       <c r="O126" s="9"/>
       <c r="P126" s="9"/>
-      <c r="Q126" s="9"/>
     </row>
     <row r="127" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C127" s="6"/>
@@ -2461,7 +2240,6 @@
       <c r="N127" s="9"/>
       <c r="O127" s="9"/>
       <c r="P127" s="9"/>
-      <c r="Q127" s="9"/>
     </row>
     <row r="128" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C128" s="6"/>
@@ -2476,7 +2254,6 @@
       <c r="N128" s="9"/>
       <c r="O128" s="9"/>
       <c r="P128" s="9"/>
-      <c r="Q128" s="9"/>
     </row>
     <row r="129" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C129" s="6"/>
@@ -2491,7 +2268,6 @@
       <c r="N129" s="9"/>
       <c r="O129" s="9"/>
       <c r="P129" s="9"/>
-      <c r="Q129" s="9"/>
     </row>
     <row r="130" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C130" s="6"/>
@@ -2506,7 +2282,6 @@
       <c r="N130" s="9"/>
       <c r="O130" s="9"/>
       <c r="P130" s="9"/>
-      <c r="Q130" s="9"/>
     </row>
     <row r="131" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C131" s="6"/>
@@ -2521,7 +2296,6 @@
       <c r="N131" s="9"/>
       <c r="O131" s="9"/>
       <c r="P131" s="9"/>
-      <c r="Q131" s="9"/>
     </row>
     <row r="132" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C132" s="6"/>
@@ -2536,7 +2310,6 @@
       <c r="N132" s="9"/>
       <c r="O132" s="9"/>
       <c r="P132" s="9"/>
-      <c r="Q132" s="9"/>
     </row>
     <row r="133" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C133" s="6"/>
@@ -2551,7 +2324,6 @@
       <c r="N133" s="9"/>
       <c r="O133" s="9"/>
       <c r="P133" s="9"/>
-      <c r="Q133" s="9"/>
     </row>
     <row r="134" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C134" s="6"/>
@@ -2565,7 +2337,6 @@
       <c r="M134" s="8"/>
       <c r="N134" s="9"/>
       <c r="O134" s="9"/>
-      <c r="P134" s="9"/>
     </row>
     <row r="135" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C135" s="6"/>
@@ -2579,7 +2350,6 @@
       <c r="M135" s="8"/>
       <c r="N135" s="9"/>
       <c r="O135" s="9"/>
-      <c r="P135" s="9"/>
     </row>
     <row r="136" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C136" s="6"/>
@@ -2593,7 +2363,6 @@
       <c r="M136" s="8"/>
       <c r="N136" s="9"/>
       <c r="O136" s="9"/>
-      <c r="P136" s="9"/>
     </row>
     <row r="137" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C137" s="6"/>
@@ -2607,7 +2376,6 @@
       <c r="M137" s="8"/>
       <c r="N137" s="9"/>
       <c r="O137" s="9"/>
-      <c r="P137" s="9"/>
     </row>
     <row r="138" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C138" s="6"/>
@@ -2621,7 +2389,6 @@
       <c r="M138" s="8"/>
       <c r="N138" s="9"/>
       <c r="O138" s="9"/>
-      <c r="P138" s="9"/>
     </row>
     <row r="139" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C139" s="6"/>
@@ -2635,7 +2402,6 @@
       <c r="M139" s="8"/>
       <c r="N139" s="9"/>
       <c r="O139" s="9"/>
-      <c r="P139" s="9"/>
     </row>
     <row r="140" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C140" s="6"/>
@@ -2649,7 +2415,6 @@
       <c r="M140" s="8"/>
       <c r="N140" s="9"/>
       <c r="O140" s="9"/>
-      <c r="P140" s="9"/>
     </row>
     <row r="141" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C141" s="6"/>
@@ -2663,7 +2428,6 @@
       <c r="M141" s="8"/>
       <c r="N141" s="9"/>
       <c r="O141" s="9"/>
-      <c r="P141" s="9"/>
     </row>
     <row r="142" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C142" s="6"/>
@@ -2677,7 +2441,6 @@
       <c r="M142" s="8"/>
       <c r="N142" s="9"/>
       <c r="O142" s="9"/>
-      <c r="P142" s="9"/>
     </row>
     <row r="143" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C143" s="6"/>
@@ -2691,7 +2454,6 @@
       <c r="M143" s="8"/>
       <c r="N143" s="9"/>
       <c r="O143" s="9"/>
-      <c r="P143" s="9"/>
     </row>
     <row r="144" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C144" s="6"/>
@@ -2705,7 +2467,6 @@
       <c r="M144" s="8"/>
       <c r="N144" s="9"/>
       <c r="O144" s="9"/>
-      <c r="P144" s="9"/>
     </row>
     <row r="145" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C145" s="6"/>
@@ -2719,7 +2480,6 @@
       <c r="M145" s="8"/>
       <c r="N145" s="9"/>
       <c r="O145" s="9"/>
-      <c r="P145" s="9"/>
     </row>
     <row r="146" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C146" s="6"/>
@@ -2733,7 +2493,6 @@
       <c r="M146" s="8"/>
       <c r="N146" s="9"/>
       <c r="O146" s="9"/>
-      <c r="P146" s="9"/>
     </row>
     <row r="147" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C147" s="6"/>
@@ -2747,7 +2506,6 @@
       <c r="M147" s="8"/>
       <c r="N147" s="9"/>
       <c r="O147" s="9"/>
-      <c r="P147" s="9"/>
     </row>
     <row r="148" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C148" s="6"/>
@@ -2761,7 +2519,6 @@
       <c r="M148" s="8"/>
       <c r="N148" s="9"/>
       <c r="O148" s="9"/>
-      <c r="P148" s="9"/>
     </row>
     <row r="149" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C149" s="6"/>
@@ -2775,7 +2532,6 @@
       <c r="M149" s="8"/>
       <c r="N149" s="9"/>
       <c r="O149" s="9"/>
-      <c r="P149" s="9"/>
     </row>
     <row r="150" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C150" s="6"/>
@@ -2789,7 +2545,6 @@
       <c r="M150" s="8"/>
       <c r="N150" s="9"/>
       <c r="O150" s="9"/>
-      <c r="P150" s="9"/>
     </row>
     <row r="151" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C151" s="6"/>
@@ -2803,7 +2558,6 @@
       <c r="M151" s="8"/>
       <c r="N151" s="9"/>
       <c r="O151" s="9"/>
-      <c r="P151" s="9"/>
     </row>
     <row r="152" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C152" s="6"/>
@@ -2817,7 +2571,6 @@
       <c r="M152" s="8"/>
       <c r="N152" s="9"/>
       <c r="O152" s="9"/>
-      <c r="P152" s="9"/>
     </row>
     <row r="153" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C153" s="6"/>
@@ -2831,7 +2584,6 @@
       <c r="M153" s="8"/>
       <c r="N153" s="9"/>
       <c r="O153" s="9"/>
-      <c r="P153" s="9"/>
     </row>
     <row r="154" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C154" s="6"/>
@@ -2845,7 +2597,6 @@
       <c r="M154" s="8"/>
       <c r="N154" s="9"/>
       <c r="O154" s="9"/>
-      <c r="P154" s="9"/>
     </row>
     <row r="155" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C155" s="6"/>
@@ -2859,7 +2610,6 @@
       <c r="M155" s="8"/>
       <c r="N155" s="9"/>
       <c r="O155" s="9"/>
-      <c r="P155" s="9"/>
     </row>
     <row r="156" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C156" s="6"/>
@@ -2873,7 +2623,6 @@
       <c r="M156" s="8"/>
       <c r="N156" s="9"/>
       <c r="O156" s="9"/>
-      <c r="P156" s="9"/>
     </row>
     <row r="157" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C157" s="6"/>
@@ -2887,7 +2636,6 @@
       <c r="M157" s="8"/>
       <c r="N157" s="9"/>
       <c r="O157" s="9"/>
-      <c r="P157" s="9"/>
     </row>
     <row r="158" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C158" s="6"/>
@@ -2901,7 +2649,6 @@
       <c r="M158" s="8"/>
       <c r="N158" s="9"/>
       <c r="O158" s="9"/>
-      <c r="P158" s="9"/>
     </row>
     <row r="159" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C159" s="6"/>
@@ -2915,7 +2662,6 @@
       <c r="M159" s="8"/>
       <c r="N159" s="9"/>
       <c r="O159" s="9"/>
-      <c r="P159" s="9"/>
     </row>
     <row r="160" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C160" s="6"/>
@@ -2929,7 +2675,6 @@
       <c r="M160" s="8"/>
       <c r="N160" s="9"/>
       <c r="O160" s="9"/>
-      <c r="P160" s="9"/>
     </row>
     <row r="161" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C161" s="6"/>
@@ -2943,7 +2688,6 @@
       <c r="M161" s="8"/>
       <c r="N161" s="9"/>
       <c r="O161" s="9"/>
-      <c r="P161" s="9"/>
     </row>
     <row r="162" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C162" s="6"/>
@@ -2957,7 +2701,6 @@
       <c r="M162" s="8"/>
       <c r="N162" s="9"/>
       <c r="O162" s="9"/>
-      <c r="P162" s="9"/>
     </row>
     <row r="163" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C163" s="6"/>
@@ -2971,7 +2714,6 @@
       <c r="M163" s="8"/>
       <c r="N163" s="9"/>
       <c r="O163" s="9"/>
-      <c r="P163" s="9"/>
     </row>
     <row r="164" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C164" s="6"/>
@@ -2985,7 +2727,6 @@
       <c r="M164" s="8"/>
       <c r="N164" s="9"/>
       <c r="O164" s="9"/>
-      <c r="P164" s="9"/>
     </row>
     <row r="165" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C165" s="6"/>
@@ -2999,7 +2740,6 @@
       <c r="M165" s="8"/>
       <c r="N165" s="9"/>
       <c r="O165" s="9"/>
-      <c r="P165" s="9"/>
     </row>
     <row r="166" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C166" s="6"/>
@@ -3013,7 +2753,6 @@
       <c r="M166" s="8"/>
       <c r="N166" s="9"/>
       <c r="O166" s="9"/>
-      <c r="P166" s="9"/>
     </row>
     <row r="167" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C167" s="6"/>
@@ -3027,7 +2766,6 @@
       <c r="M167" s="8"/>
       <c r="N167" s="9"/>
       <c r="O167" s="9"/>
-      <c r="P167" s="9"/>
     </row>
     <row r="168" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C168" s="6"/>
@@ -3041,7 +2779,6 @@
       <c r="M168" s="8"/>
       <c r="N168" s="9"/>
       <c r="O168" s="9"/>
-      <c r="P168" s="9"/>
     </row>
     <row r="169" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C169" s="6"/>
@@ -3055,7 +2792,6 @@
       <c r="M169" s="8"/>
       <c r="N169" s="9"/>
       <c r="O169" s="9"/>
-      <c r="P169" s="9"/>
     </row>
     <row r="170" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C170" s="6"/>
@@ -3069,7 +2805,6 @@
       <c r="M170" s="8"/>
       <c r="N170" s="9"/>
       <c r="O170" s="9"/>
-      <c r="P170" s="9"/>
     </row>
     <row r="171" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C171" s="6"/>
@@ -3083,7 +2818,6 @@
       <c r="M171" s="8"/>
       <c r="N171" s="9"/>
       <c r="O171" s="9"/>
-      <c r="P171" s="9"/>
     </row>
     <row r="172" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C172" s="6"/>
@@ -3097,7 +2831,6 @@
       <c r="M172" s="8"/>
       <c r="N172" s="9"/>
       <c r="O172" s="9"/>
-      <c r="P172" s="9"/>
     </row>
     <row r="173" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C173" s="6"/>
@@ -3111,7 +2844,6 @@
       <c r="M173" s="8"/>
       <c r="N173" s="9"/>
       <c r="O173" s="9"/>
-      <c r="P173" s="9"/>
     </row>
     <row r="174" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C174" s="6"/>
@@ -3125,7 +2857,6 @@
       <c r="M174" s="8"/>
       <c r="N174" s="9"/>
       <c r="O174" s="9"/>
-      <c r="P174" s="9"/>
     </row>
     <row r="175" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C175" s="6"/>
@@ -3887,12 +3618,12 @@
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>31</v>
+        <v>35</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>